<commit_message>
Beschleunigung in excel files von Mittlerer Geschwindigkeit und
</commit_message>
<xml_diff>
--- a/Versuch6/datasets/mittlere_geschwindigkeit.xlsx
+++ b/Versuch6/datasets/mittlere_geschwindigkeit.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Uni\Grundpraktikum\Versuch6\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4AE97A3-7763-4CE1-AAC8-09A3C4505D9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A747F9CA-9000-4F52-A994-C0BB3A56F5E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22932" windowHeight="5616" xr2:uid="{77E49A20-21DB-4605-A4AB-B0C3445176E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22932" windowHeight="5616" activeTab="1" xr2:uid="{77E49A20-21DB-4605-A4AB-B0C3445176E8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mittlere Geschwindigkeit" sheetId="1" r:id="rId1"/>
+    <sheet name="Direkte Messung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>d</t>
   </si>
@@ -48,9 +49,6 @@
     <t>d_err</t>
   </si>
   <si>
-    <t>speed_dev</t>
-  </si>
-  <si>
     <t>t_dev</t>
   </si>
   <si>
@@ -63,9 +61,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>shreiben</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -76,6 +71,24 @@
   </si>
   <si>
     <t>v_avg</t>
+  </si>
+  <si>
+    <t>v_corr_avg</t>
+  </si>
+  <si>
+    <t>v_err_avg</t>
+  </si>
+  <si>
+    <t>delta_x</t>
+  </si>
+  <si>
+    <t>delta_x_err</t>
+  </si>
+  <si>
+    <t>a_err</t>
+  </si>
+  <si>
+    <t>a_corr</t>
   </si>
 </sst>
 </file>
@@ -427,18 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09242045-FE9D-4060-BF77-9A857490A3AF}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.88671875" customWidth="1"/>
+    <col min="14" max="15" width="10.77734375" customWidth="1"/>
+    <col min="19" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,31 +476,28 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
+      <c r="K1" t="s">
+        <v>11</v>
       </c>
       <c r="L1" t="s">
         <v>13</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>140</v>
       </c>
@@ -519,26 +531,20 @@
         <f>_xlfn.STDEV.P(C2:G2)</f>
         <v>1.552546295606048E-3</v>
       </c>
+      <c r="K2">
+        <v>54.6</v>
+      </c>
       <c r="L2">
-        <v>56.8</v>
+        <v>0.2</v>
       </c>
       <c r="M2">
-        <f>L2*0.985</f>
-        <v>55.947999999999993</v>
+        <v>100</v>
       </c>
       <c r="N2">
-        <f>SQRT(0.1^2+(M2*3*10^(-5))^2+(M2*0.005)^2)</f>
-        <v>0.2970812763551981</v>
-      </c>
-      <c r="O2">
-        <f>AVERAGE(L2:L7)</f>
-        <v>56.666666666666664</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>120</v>
       </c>
@@ -573,24 +579,13 @@
         <f t="shared" ref="J3:J8" si="2">_xlfn.STDEV.P(C3:G3)</f>
         <v>9.3680307429039843E-4</v>
       </c>
-      <c r="L3">
-        <v>56.4</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M7" si="3">L3*0.985</f>
-        <v>55.553999999999995</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N7" si="4">SQRT(0.1^2+(M3*3*10^(-5))^2+(M3*0.005)^2)</f>
-        <v>0.29522694748654699</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B8" si="5">B3</f>
+        <f t="shared" ref="B4:B8" si="3">B3</f>
         <v>0.5</v>
       </c>
       <c r="C4">
@@ -620,27 +615,19 @@
         <f t="shared" si="2"/>
         <v>1.097998178504902E-3</v>
       </c>
-      <c r="L4">
-        <v>56.4</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>55.553999999999995</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="4"/>
-        <v>0.29522694748654699</v>
-      </c>
-      <c r="O4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80</v>
       </c>
       <c r="B5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C5">
@@ -670,28 +657,21 @@
         <f t="shared" si="2"/>
         <v>9.0686272390035311E-4</v>
       </c>
-      <c r="L5">
-        <v>56.8</v>
-      </c>
       <c r="M5">
-        <f t="shared" si="3"/>
-        <v>55.947999999999993</v>
+        <f>0.5*K2^2/M2</f>
+        <v>14.905800000000001</v>
       </c>
       <c r="N5">
-        <f t="shared" si="4"/>
-        <v>0.2970812763551981</v>
-      </c>
-      <c r="O5">
-        <f>_xlfn.STDEV.S(L2:L7)</f>
-        <v>0.20655911179772815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <f>SQRT(K2^2*L2^2/(M2^2)+K2^4*N2^2/(4*M2^4))</f>
+        <v>0.13220897034997287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60</v>
       </c>
       <c r="B6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C6">
@@ -721,24 +701,13 @@
         <f t="shared" si="2"/>
         <v>4.270831300812616E-4</v>
       </c>
-      <c r="L6">
-        <v>56.8</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>55.947999999999993</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>0.2970812763551981</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>40</v>
       </c>
       <c r="B7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C7">
@@ -768,24 +737,13 @@
         <f t="shared" si="2"/>
         <v>2.5768197453451895E-4</v>
       </c>
-      <c r="L7">
-        <v>56.8</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>55.947999999999993</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="4"/>
-        <v>0.2970812763551981</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C8">
@@ -822,4 +780,167 @@
     <ignoredError sqref="H2 H3:J8 I2:J2" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91984ABA-8172-431F-BD86-03353843578B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>56.8</v>
+      </c>
+      <c r="D2">
+        <f>C2*0.985</f>
+        <v>55.947999999999993</v>
+      </c>
+      <c r="E2">
+        <f>SQRT(0.1^2+(D2*3*10^(-5))^2+(D2*0.005)^2)</f>
+        <v>0.2970812763551981</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(C2:C7)</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="G2">
+        <f>0.5*F2^2/A2</f>
+        <v>16.055555555555554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>56.4</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="0">C3*0.985</f>
+        <v>55.553999999999995</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="1">SQRT(0.1^2+(D3*3*10^(-5))^2+(D3*0.005)^2)</f>
+        <v>0.29522694748654699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>56.4</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>55.553999999999995</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.29522694748654699</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>56.8</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>55.947999999999993</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.2970812763551981</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(D2:D7)</f>
+        <v>55.816666666666656</v>
+      </c>
+      <c r="G5">
+        <f>0.5*F5^2/A2</f>
+        <v>15.577501388888884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>56.8</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>55.947999999999993</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.2970812763551981</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>56.8</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>55.947999999999993</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0.2970812763551981</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f>AVERAGE(E2:E7)</f>
+        <v>0.29646316673231438</v>
+      </c>
+      <c r="G8">
+        <f>SQRT(F2^2*F8^2/A2^2+F2^4*B2^2/(4*A2^4))</f>
+        <v>0.18619105394314009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>